<commit_message>
hopefully got rd2rus to run...
</commit_message>
<xml_diff>
--- a/6_app/API_endpoints_v1.1.xlsx
+++ b/6_app/API_endpoints_v1.1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11480" yWindow="880" windowWidth="31560" windowHeight="19300" tabRatio="500"/>
+    <workbookView xWindow="6840" yWindow="480" windowWidth="31560" windowHeight="19300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="endpoints" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="142">
   <si>
     <t>type</t>
   </si>
@@ -433,13 +433,28 @@
     <t>^eg</t>
   </si>
   <si>
-    <t>need to make file</t>
-  </si>
-  <si>
     <t>route_ID</t>
   </si>
   <si>
     <t>number_pitches</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>Route_file format</t>
+  </si>
+  <si>
+    <t>RUS_file format</t>
+  </si>
+  <si>
+    <t>user_ID</t>
+  </si>
+  <si>
+    <t>stars</t>
+  </si>
+  <si>
+    <t>estimated stars</t>
   </si>
 </sst>
 </file>
@@ -472,12 +487,24 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -492,7 +519,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -500,6 +527,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -777,38 +807,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:J6"/>
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="43.33203125" customWidth="1"/>
     <col min="6" max="10" width="15.33203125" customWidth="1"/>
+    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>134</v>
-      </c>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="N3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -816,7 +859,7 @@
         <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G4" t="s">
         <v>10</v>
@@ -828,10 +871,28 @@
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+      <c r="K4" t="s">
+        <v>135</v>
+      </c>
+      <c r="L4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N4" t="s">
+        <v>134</v>
+      </c>
+      <c r="O4" t="s">
+        <v>139</v>
+      </c>
+      <c r="P4" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -839,7 +900,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -847,7 +908,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -855,46 +916,46 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B8" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>136</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>129</v>
       </c>
@@ -902,7 +963,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -910,44 +971,62 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>10</v>
       </c>
       <c r="B24" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="K24">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>11</v>
       </c>
       <c r="B25" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="K25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B26" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="K26">
+        <f>K24/K25</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>12</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="K27">
+        <f>K26*3</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>15</v>
       </c>
       <c r="B28" t="s">
         <v>16</v>
+      </c>
+      <c r="K28">
+        <f>K27/3600</f>
+        <v>0.83333333333333337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>